<commit_message>
Added bandpower PCA analysis
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\etc\uni\yr5\project\workspace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\etc\uni\yr5\project\workspace\eeg-cnp-final-year-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50556FD9-FBEE-41DE-A809-2737321EB280}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3C5918-E5E7-4458-B78C-1E0AAAC2E807}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1488" yWindow="468" windowWidth="18900" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
   <si>
     <t>Method</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>nu = 0.70094, n_clusters=5</t>
+  </si>
+  <si>
+    <t>0, 0, 2, 11, 19, 33, 33, 33, 33, 36, 37, 37, 39, 43, 43, 43, 49, 49, 50</t>
+  </si>
+  <si>
+    <t>k = 27; freq bands (Hz) 4-7, 8-12, 13-30</t>
   </si>
 </sst>
 </file>
@@ -527,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,10 +631,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>0.86460000000000004</v>
+        <v>0.84340000000000004</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -637,10 +643,10 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -648,19 +654,19 @@
         <v>16</v>
       </c>
       <c r="B6" s="1">
-        <v>0.88449999999999995</v>
+        <v>0.86460000000000004</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -668,19 +674,19 @@
         <v>16</v>
       </c>
       <c r="B7" s="1">
-        <v>0.86970000000000003</v>
+        <v>0.88449999999999995</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -688,7 +694,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="1">
-        <v>0.89710000000000001</v>
+        <v>0.86970000000000003</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -697,10 +703,10 @@
         <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -708,7 +714,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="1">
-        <v>0.90100000000000002</v>
+        <v>0.89710000000000001</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -717,10 +723,10 @@
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -728,7 +734,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="1">
-        <v>0.88160000000000005</v>
+        <v>0.90100000000000002</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
@@ -737,10 +743,10 @@
         <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -748,99 +754,99 @@
         <v>16</v>
       </c>
       <c r="B11" s="1">
-        <v>0.89610000000000001</v>
+        <v>0.88160000000000005</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1">
-        <v>0.49419999999999997</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>34</v>
+        <v>0.89610000000000001</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="E12">
-        <v>36</v>
+      <c r="E12" t="s">
+        <v>31</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1">
-        <v>0.78080000000000005</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
+        <v>0.49419999999999997</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="E13" t="s">
-        <v>40</v>
+      <c r="E13">
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1">
-        <v>0.83009999999999995</v>
+        <v>0.78080000000000005</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1">
-        <v>0.70650000000000002</v>
+        <v>0.83009999999999995</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -848,98 +854,118 @@
         <v>41</v>
       </c>
       <c r="B16" s="1">
-        <v>0.81310000000000004</v>
+        <v>0.70650000000000002</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B17" s="1">
-        <v>0.72030000000000005</v>
+        <v>0.81310000000000004</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B18" s="1">
-        <v>0.88839999999999997</v>
+        <v>0.72030000000000005</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B19" s="1">
-        <v>0.71230000000000004</v>
+        <v>0.88839999999999997</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.71230000000000004</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B21" s="1">
         <v>0.78649999999999998</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>7</v>
       </c>
-      <c r="D20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
         <v>59</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F21" t="s">
         <v>60</v>
       </c>
     </row>
@@ -947,7 +973,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C12" twoDigitTextYear="1"/>
+    <ignoredError sqref="C13" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More bandpower PCA experiments
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\etc\uni\yr5\project\workspace\eeg-cnp-final-year-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3C5918-E5E7-4458-B78C-1E0AAAC2E807}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FE7D79-37DF-4116-A77D-EB5566F8B83C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
   <si>
     <t>Method</t>
   </si>
@@ -214,6 +214,18 @@
   </si>
   <si>
     <t>k = 27; freq bands (Hz) 4-7, 8-12, 13-30</t>
+  </si>
+  <si>
+    <t>Bandpower + PCA + NuSVM (linear kernel)</t>
+  </si>
+  <si>
+    <t>19/19</t>
+  </si>
+  <si>
+    <t>0, 1, 1, 2, 3, 3, 5, 12, 13, 23, 30, 52, 57</t>
+  </si>
+  <si>
+    <t>nu=8585, n_components=3, freq bands (Hz) 4-8,8-13,13-30</t>
   </si>
 </sst>
 </file>
@@ -533,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -969,6 +981,26 @@
         <v>60</v>
       </c>
     </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.96050000000000002</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Further experiments with HFD: k variation, half-sampling rate
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\etc\uni\yr5\project\workspace\eeg-cnp-final-year-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FE7D79-37DF-4116-A77D-EB5566F8B83C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324D36DE-FD7C-45A9-BF71-19A4A18EC29C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="20688" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="68">
   <si>
     <t>Method</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>nu=8585, n_components=3, freq bands (Hz) 4-8,8-13,13-30</t>
+  </si>
+  <si>
+    <t>nu = 0.25007, HFD over 375-500</t>
   </si>
 </sst>
 </file>
@@ -545,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -903,101 +906,121 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1">
-        <v>0.72030000000000005</v>
+        <v>0.83489999999999998</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
-      <c r="E18" t="s">
-        <v>49</v>
+      <c r="E18">
+        <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B19" s="1">
-        <v>0.88839999999999997</v>
+        <v>0.72030000000000005</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B20" s="1">
-        <v>0.71230000000000004</v>
+        <v>0.88839999999999997</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="1">
-        <v>0.78649999999999998</v>
+        <v>0.71230000000000004</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.78649999999999998</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B23" s="1">
         <v>0.96050000000000002</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>64</v>
       </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
         <v>65</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F23" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Experiments with bandpower + HFD
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\etc\uni\yr5\project\workspace\eeg-cnp-final-year-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324D36DE-FD7C-45A9-BF71-19A4A18EC29C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F31E70-DE18-45DF-A1EE-12A3F761E044}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="20688" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="70">
   <si>
     <t>Method</t>
   </si>
@@ -229,6 +229,12 @@
   </si>
   <si>
     <t>nu = 0.25007, HFD over 375-500</t>
+  </si>
+  <si>
+    <t>11, 36, 52</t>
+  </si>
+  <si>
+    <t>nu=0.8, n_components=3, freq bands (Hz) 4-8,8-13,13-30, timing 375-500</t>
   </si>
 </sst>
 </file>
@@ -548,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1024,6 +1030,26 @@
         <v>66</v>
       </c>
     </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.91869999999999996</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Plotting some graphs and figures
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\etc\uni\yr5\project\workspace\eeg-cnp-final-year-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F31E70-DE18-45DF-A1EE-12A3F761E044}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D336BB8-9CD9-48EE-A211-B6764A095B2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="20688" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1428" yWindow="492" windowWidth="20688" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="73">
   <si>
     <t>Method</t>
   </si>
@@ -235,6 +235,15 @@
   </si>
   <si>
     <t>nu=0.8, n_components=3, freq bands (Hz) 4-8,8-13,13-30, timing 375-500</t>
+  </si>
+  <si>
+    <t>Bandpower + PCA + NuSVM (poly kernel)</t>
+  </si>
+  <si>
+    <t>3, 5, 11, 13</t>
+  </si>
+  <si>
+    <t>nu=865, n_components=3, freq bands (Hz) 4-8,8-13,13-30</t>
   </si>
 </sst>
 </file>
@@ -554,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1050,6 +1059,26 @@
         <v>69</v>
       </c>
     </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.9456</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Experiments with PDP/PNP dataset
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\etc\uni\yr5\project\workspace\eeg-cnp-final-year-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D336BB8-9CD9-48EE-A211-B6764A095B2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914E852B-6E19-4EE5-A7DC-6B1BF5DF31C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1428" yWindow="492" windowWidth="20688" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="77">
   <si>
     <t>Method</t>
   </si>
@@ -244,6 +244,18 @@
   </si>
   <si>
     <t>nu=865, n_components=3, freq bands (Hz) 4-8,8-13,13-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12/12</t>
+  </si>
+  <si>
+    <t>PDP/PNP - RH</t>
+  </si>
+  <si>
+    <t>0, 3, 7, 13, 13, 13, 18, 20, 22, 24, 29, 30, 35, 46</t>
+  </si>
+  <si>
+    <t>nu=6022, n_components=3, freq bands (Hz) 4-8,8-13,13-30</t>
   </si>
 </sst>
 </file>
@@ -279,10 +291,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1079,6 +1092,26 @@
         <v>72</v>
       </c>
     </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.89870000000000005</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" t="s">
+        <v>75</v>
+      </c>
+      <c r="F26" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added legs dataset experiments
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\etc\uni\yr5\project\workspace\eeg-cnp-final-year-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914E852B-6E19-4EE5-A7DC-6B1BF5DF31C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F246642-6E36-4BD1-96F4-C10EB5B0ADA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1428" yWindow="492" windowWidth="20688" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="77">
   <si>
     <t>Method</t>
   </si>
@@ -225,9 +225,6 @@
     <t>0, 1, 1, 2, 3, 3, 5, 12, 13, 23, 30, 52, 57</t>
   </si>
   <si>
-    <t>nu=8585, n_components=3, freq bands (Hz) 4-8,8-13,13-30</t>
-  </si>
-  <si>
     <t>nu = 0.25007, HFD over 375-500</t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t>nu=6022, n_components=3, freq bands (Hz) 4-8,8-13,13-30</t>
+  </si>
+  <si>
+    <t>nu=0.8585, n_components=3, freq bands (Hz) 4-8,8-13,13-30</t>
   </si>
 </sst>
 </file>
@@ -576,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -949,7 +949,7 @@
         <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1049,7 +1049,7 @@
         <v>65</v>
       </c>
       <c r="F23" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1066,15 +1066,15 @@
         <v>12</v>
       </c>
       <c r="E24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" t="s">
         <v>68</v>
-      </c>
-      <c r="F24" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B25" s="1">
         <v>0.9456</v>
@@ -1086,10 +1086,10 @@
         <v>12</v>
       </c>
       <c r="E25" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" t="s">
         <v>71</v>
-      </c>
-      <c r="F25" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1100,15 +1100,35 @@
         <v>0.89870000000000005</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" t="s">
         <v>73</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>74</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>75</v>
       </c>
-      <c r="F26" t="s">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.84330000000000005</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>